<commit_message>
Fixes complete for first release
</commit_message>
<xml_diff>
--- a/install/import_templates/import_all.xlsx
+++ b/install/import_templates/import_all.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pegasus\install\import_templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B06A5F-A248-4C75-ADA0-1FB18C61F4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="19155" windowHeight="7770" activeTab="4"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="competitors" sheetId="2" r:id="rId1"/>
@@ -15,13 +21,14 @@
     <sheet name="rotas_help" sheetId="7" r:id="rId6"/>
     <sheet name="events" sheetId="8" r:id="rId7"/>
     <sheet name="events_help" sheetId="6" r:id="rId8"/>
+    <sheet name="race_format" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="220">
   <si>
     <t>sailnum</t>
   </si>
@@ -555,13 +562,139 @@
   </si>
   <si>
     <t>01626 444555</t>
+  </si>
+  <si>
+    <t>club_series</t>
+  </si>
+  <si>
+    <t>Fast Asymmetric</t>
+  </si>
+  <si>
+    <t>Fast Handicap</t>
+  </si>
+  <si>
+    <t>Slow Handicap</t>
+  </si>
+  <si>
+    <t>Multihull</t>
+  </si>
+  <si>
+    <t>trophy</t>
+  </si>
+  <si>
+    <t>Dinghy</t>
+  </si>
+  <si>
+    <t>SERIES</t>
+  </si>
+  <si>
+    <t>SERIES TYPW</t>
+  </si>
+  <si>
+    <t>RACE FORMATS</t>
+  </si>
+  <si>
+    <t>6-3-0</t>
+  </si>
+  <si>
+    <t>start interval</t>
+  </si>
+  <si>
+    <t>FLEET CONFIGURATION</t>
+  </si>
+  <si>
+    <t>start sequence</t>
+  </si>
+  <si>
+    <t>no. of starts</t>
+  </si>
+  <si>
+    <t>fleet no.</t>
+  </si>
+  <si>
+    <t>start no.</t>
+  </si>
+  <si>
+    <t>acronym</t>
+  </si>
+  <si>
+    <t>ASSY</t>
+  </si>
+  <si>
+    <t>FHCAP</t>
+  </si>
+  <si>
+    <t>LHCAP</t>
+  </si>
+  <si>
+    <t>MULTI</t>
+  </si>
+  <si>
+    <t>DINGHY</t>
+  </si>
+  <si>
+    <t>scoring</t>
+  </si>
+  <si>
+    <t>handicap</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>py_type</t>
+  </si>
+  <si>
+    <t>national</t>
+  </si>
+  <si>
+    <t>warning_signal</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yellow </t>
+  </si>
+  <si>
+    <t>min PY</t>
+  </si>
+  <si>
+    <t>max PY</t>
+  </si>
+  <si>
+    <t>class_inc</t>
+  </si>
+  <si>
+    <t>hull type</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>K1,Moth (foiler),Waszp</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>RS200</t>
+  </si>
+  <si>
+    <t>Moth (foiler),Waszp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,13 +733,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -618,11 +769,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -646,12 +798,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -659,6 +826,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -707,7 +877,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -740,9 +910,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -775,6 +962,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -950,7 +1154,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1106,18 +1310,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,53 +1356,53 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="13">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="11" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="13">
         <v>3718</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1271,16 +1475,19 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="D11" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1313,19 +1520,19 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="11" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1450,7 +1657,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1"/>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1458,11 +1665,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,7 +1683,8 @@
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="11" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1621,11 +1829,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,41 +1872,42 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="11" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="13">
         <v>991</v>
       </c>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1718,122 +1927,122 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="11" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="13">
         <v>1</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="11" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="11" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="11" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1881,10 +2090,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -1999,15 +2208,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2211,7 +2420,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1"/>
+    <hyperlink ref="E9" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2219,7 +2428,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2239,7 +2448,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2250,4 +2459,285 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116729DF-6578-4C52-A028-88E9400BD068}">
+  <dimension ref="A1:P18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="16" max="16" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="15">
+        <v>4</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="15">
+        <v>2</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="M5" t="s">
+        <v>214</v>
+      </c>
+      <c r="N5" t="s">
+        <v>211</v>
+      </c>
+      <c r="O5" t="s">
+        <v>212</v>
+      </c>
+      <c r="P5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H6" t="s">
+        <v>207</v>
+      </c>
+      <c r="M6" t="s">
+        <v>97</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F7" t="s">
+        <v>202</v>
+      </c>
+      <c r="G7" t="s">
+        <v>205</v>
+      </c>
+      <c r="H7" t="s">
+        <v>208</v>
+      </c>
+      <c r="M7" t="s">
+        <v>97</v>
+      </c>
+      <c r="P7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8" t="s">
+        <v>202</v>
+      </c>
+      <c r="G8" t="s">
+        <v>205</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" t="s">
+        <v>97</v>
+      </c>
+      <c r="P8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G9" t="s">
+        <v>205</v>
+      </c>
+      <c r="H9" t="s">
+        <v>209</v>
+      </c>
+      <c r="M9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>200</v>
+      </c>
+      <c r="F11" t="s">
+        <v>203</v>
+      </c>
+      <c r="G11" t="s">
+        <v>205</v>
+      </c>
+      <c r="H11" t="s">
+        <v>210</v>
+      </c>
+      <c r="M11" t="s">
+        <v>97</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1300</v>
+      </c>
+      <c r="P11" s="17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>199</v>
+      </c>
+      <c r="F12" t="s">
+        <v>203</v>
+      </c>
+      <c r="G12" t="s">
+        <v>205</v>
+      </c>
+      <c r="H12" t="s">
+        <v>208</v>
+      </c>
+      <c r="M12" t="s">
+        <v>215</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>